<commit_message>
3eme commit, ajout de filtre
</commit_message>
<xml_diff>
--- a/truc à faire.xlsx
+++ b/truc à faire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cegep\projet_perso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F0A1F-B65A-457B-A76F-B6D7C403F7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0271BB5B-F344-44E1-97DC-6FAEE2AE1AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2124" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKEND" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>ajout deck</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>afficher les decks et leur détails</t>
+  </si>
+  <si>
+    <t>creation compte</t>
+  </si>
+  <si>
+    <t>demande au prof pour le dossier dev des test</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADE521A-B2DE-4C37-8D86-1F00223CA5D2}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,6 +641,16 @@
         <v>21</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
projet fini dans l'ensemble, reste les commentaires à ajouter et les messages derreur à vérifier
</commit_message>
<xml_diff>
--- a/truc à faire.xlsx
+++ b/truc à faire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cegep\projet_perso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0271BB5B-F344-44E1-97DC-6FAEE2AE1AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D63E505-8A55-45CA-988D-EA7DF796AA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2124" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKEND" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>ajout deck</t>
   </si>
@@ -107,6 +107,21 @@
   </si>
   <si>
     <t>demande au prof pour le dossier dev des test</t>
+  </si>
+  <si>
+    <t>faire un readme pour starter le projet</t>
+  </si>
+  <si>
+    <t>faire les commentaires</t>
+  </si>
+  <si>
+    <t>vérifier les messages d'erreur</t>
+  </si>
+  <si>
+    <t>faire le tour du site pour trouver des erreurs</t>
+  </si>
+  <si>
+    <t>faire le fichier txt qui explique ce que chaque test fait</t>
   </si>
 </sst>
 </file>
@@ -424,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,6 +554,21 @@
         <v>21</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -546,10 +576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADE521A-B2DE-4C37-8D86-1F00223CA5D2}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,16 +631,25 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -624,6 +663,9 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -645,10 +687,36 @@
       <c r="A13" t="s">
         <v>25</v>
       </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>